<commit_message>
fixing tests for xlsx - replacing && by and - separating subsequent conditional statements
</commit_message>
<xml_diff>
--- a/tests/data/xls/E_CZ_T2C_authoring.xlsx
+++ b/tests/data/xls/E_CZ_T2C_authoring.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF85B04-841C-4589-85B5-D45B617A00A5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5CBE69-2FB4-4F94-B507-8FF5451CBD64}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15336" windowHeight="3744" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -423,9 +423,6 @@
     <t>// Pokud chcete omezit podmínku, můžete přidat podmínku, že je zároveň rozpoznán i nějaký intent např.</t>
   </si>
   <si>
-    <t>#BOLEST &amp;&amp; @KONCETINA:ruka</t>
-  </si>
-  <si>
     <t>// Podobne lze zapisovat podobný typ otázek. Velmi často se například objevují otázky typu "Co je to  xxx", otázka má řadu variant např. "Vysvětlete mi prosím xxx" a předmět dotazu také. </t>
   </si>
   <si>
@@ -450,19 +447,10 @@
     <t>rentgen;RTG</t>
   </si>
   <si>
-    <t>#CO_JE &amp;&amp; @PREDMET:CT</t>
-  </si>
-  <si>
     <t xml:space="preserve">Počítačová (computerová) tomografie kombinuje klasické rentgenové vyšetřením s počítačovým systémem, který informace zpracovává. </t>
   </si>
   <si>
-    <t>#CO_JE &amp;&amp; @PREDMET:rentgen</t>
-  </si>
-  <si>
     <t>// Pokud má entita velké množství položek, je přehlednější následující formát zápisu</t>
-  </si>
-  <si>
-    <t>#CO_JE &amp;&amp; @PREDMET:&lt;x&gt;</t>
   </si>
   <si>
     <t>rentgen</t>
@@ -758,13 +746,25 @@
     <t xml:space="preserve"> @KONCETINA</t>
   </si>
   <si>
-    <t xml:space="preserve"> true &amp;&amp; @KONCETINA:ruka </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> true &amp;&amp; @KONCETINA:noha</t>
-  </si>
-  <si>
     <t>//  'true &amp;&amp;' je docasna oprava chyby v detekci podmínky, po jejím opravení nebude potřeba</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @KONCETINA:ruka </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @KONCETINA:noha</t>
+  </si>
+  <si>
+    <t>#BOLEST and @KONCETINA:ruka</t>
+  </si>
+  <si>
+    <t>#CO_JE and @PREDMET:CT</t>
+  </si>
+  <si>
+    <t>#CO_JE and @PREDMET:rentgen</t>
+  </si>
+  <si>
+    <t>#CO_JE and @PREDMET:&lt;x&gt;</t>
   </si>
 </sst>
 </file>
@@ -1192,10 +1192,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D208"/>
+  <dimension ref="A1:D209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="A141" sqref="A141"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="A178" sqref="A178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1217,7 +1217,7 @@
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1227,7 +1227,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1288,7 +1288,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -1348,7 +1348,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1486,10 +1486,10 @@
         <v>44</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -1500,7 +1500,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="8" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
@@ -1508,7 +1508,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="8" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B58" s="9" t="s">
         <v>45</v>
@@ -1524,7 +1524,7 @@
     </row>
     <row r="60" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B60" s="9" t="s">
         <v>46</v>
@@ -1533,7 +1533,7 @@
         <v>47</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -1544,7 +1544,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="8" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="8"/>
@@ -1578,27 +1578,27 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="68" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="16" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="69" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="16" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="16" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="16" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
@@ -1942,7 +1942,7 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="8" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B129" s="8"/>
       <c r="C129" s="8"/>
@@ -2002,7 +2002,7 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="8" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B141" s="8" t="s">
         <v>105</v>
@@ -2010,62 +2010,54 @@
       <c r="C141" s="8"/>
       <c r="D141" s="8"/>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A142" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="B142" s="8" t="s">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A143" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B143" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="C142" s="8"/>
-      <c r="D142" s="8"/>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A143" t="s">
-        <v>180</v>
-      </c>
+      <c r="C143" s="8"/>
+      <c r="D143" s="8"/>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>107</v>
+        <v>174</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A147" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="B147" s="8" t="s">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A148" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B148" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="C147" s="8"/>
-      <c r="D147" s="8"/>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A149" t="s">
-        <v>110</v>
-      </c>
+      <c r="C148" s="8"/>
+      <c r="D148" s="8"/>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A152" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="B152" s="8"/>
-      <c r="C152" s="8"/>
-      <c r="D152" s="8"/>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" s="8" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="B153" s="8"/>
       <c r="C153" s="8"/>
@@ -2073,7 +2065,7 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" s="8" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="B154" s="8"/>
       <c r="C154" s="8"/>
@@ -2081,29 +2073,29 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B155" s="8"/>
       <c r="C155" s="8"/>
       <c r="D155" s="8"/>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A156" s="8"/>
+      <c r="A156" s="8" t="s">
+        <v>113</v>
+      </c>
       <c r="B156" s="8"/>
       <c r="C156" s="8"/>
       <c r="D156" s="8"/>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A157" s="8" t="s">
-        <v>115</v>
-      </c>
+      <c r="A157" s="8"/>
       <c r="B157" s="8"/>
       <c r="C157" s="8"/>
       <c r="D157" s="8"/>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B158" s="8"/>
       <c r="C158" s="8"/>
@@ -2111,280 +2103,288 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B159" s="8"/>
       <c r="C159" s="8"/>
       <c r="D159" s="8"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A160" s="8"/>
+      <c r="A160" s="8" t="s">
+        <v>116</v>
+      </c>
       <c r="B160" s="8"/>
       <c r="C160" s="8"/>
       <c r="D160" s="8"/>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A161" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B161" s="8" t="s">
-        <v>119</v>
-      </c>
+      <c r="A161" s="8"/>
+      <c r="B161" s="8"/>
       <c r="C161" s="8"/>
       <c r="D161" s="8"/>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A162" s="8"/>
-      <c r="B162" s="8"/>
+      <c r="A162" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="B162" s="8" t="s">
+        <v>117</v>
+      </c>
       <c r="C162" s="8"/>
       <c r="D162" s="8"/>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A163" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="B163" s="8" t="s">
-        <v>90</v>
-      </c>
+      <c r="A163" s="8"/>
+      <c r="B163" s="8"/>
       <c r="C163" s="8"/>
       <c r="D163" s="8"/>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A165" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A167" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="B167" s="8"/>
-      <c r="C167" s="8"/>
-      <c r="D167" s="8"/>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A164" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B164" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C164" s="8"/>
+      <c r="D164" s="8"/>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="B168" s="8" t="s">
-        <v>119</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="B168" s="8"/>
       <c r="C168" s="8"/>
       <c r="D168" s="8"/>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" s="8" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B169" s="8" t="s">
-        <v>90</v>
+        <v>117</v>
       </c>
       <c r="C169" s="8"/>
       <c r="D169" s="8"/>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A171" s="16" t="s">
-        <v>154</v>
-      </c>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A170" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B170" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C170" s="8"/>
+      <c r="D170" s="8"/>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" s="16" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" s="16" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" s="16" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" s="16" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" s="16" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" s="16" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" s="16" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" s="16" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" s="16" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" s="16" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" s="16" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" s="16" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A184" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="B184" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="C184" s="8"/>
-      <c r="D184" s="8"/>
+      <c r="A184" s="16" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A185" s="16" t="s">
-        <v>157</v>
-      </c>
+      <c r="A185" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B185" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C185" s="8"/>
+      <c r="D185" s="8"/>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A186" s="16"/>
+      <c r="A186" s="16" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A187" s="16" t="s">
-        <v>128</v>
-      </c>
+      <c r="A187" s="16"/>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" s="16" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A189" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="B189" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="C189" s="8"/>
-      <c r="D189" s="8"/>
+      <c r="A189" s="16" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A190" s="15"/>
-      <c r="B190" s="15"/>
-      <c r="C190" s="15"/>
-      <c r="D190" s="15"/>
+      <c r="A190" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B190" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="C190" s="8"/>
+      <c r="D190" s="8"/>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A191" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="B191" s="15" t="s">
-        <v>168</v>
-      </c>
+      <c r="A191" s="15"/>
+      <c r="B191" s="15"/>
       <c r="C191" s="15"/>
       <c r="D191" s="15"/>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A192" s="15"/>
-      <c r="B192" s="15"/>
+      <c r="A192" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="B192" s="15" t="s">
+        <v>164</v>
+      </c>
       <c r="C192" s="15"/>
       <c r="D192" s="15"/>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A193" s="16" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A194" s="16"/>
-    </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A195" s="16" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A193" s="15"/>
+      <c r="B193" s="15"/>
+      <c r="C193" s="15"/>
+      <c r="D193" s="15"/>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A194" s="16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A195" s="16"/>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A197" s="16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A198" s="16" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A199" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="B199" s="15" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A200" s="16"/>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A201" s="16" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="197" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A197" s="16" t="s">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A202" s="16" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A203" s="16" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A204" s="16" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="198" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A198" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="B198" s="15" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A199" s="16"/>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A200" s="16" t="s">
+    <row r="205" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A205" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="B205" s="15" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A201" s="16" t="s">
+    <row r="206" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="207" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A207" s="15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A208" s="15" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A202" s="16" t="s">
+      <c r="B208" s="15" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A203" s="16" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="204" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A204" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="B204" s="15" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="205" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="206" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A206" s="15" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="207" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A207" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="B207" s="15" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A208" s="16"/>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A209" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>